<commit_message>
第二季11课时.冒险关卡创建怪物   1.DlgAdventureSystem.OnStartGameLevelClickHandler 调用 AdventureHelper.RequestStartGameLevel 成功   2.AdventureComponentSystem StartAdventure()  CreateAdventureEnemy()   3.根据关卡ID读取配置表创建怪物 UnitFactory.CreateMonster
</commit_message>
<xml_diff>
--- a/Excel/BattleLevelConfig@cs.xlsx
+++ b/Excel/BattleLevelConfig@cs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Project\UnityProject\ETGameLesson\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Unity\Project\ET-EUI-Study\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AFBC696-DB43-4336-BE1F-7BA82FF68537}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FD1D9AF-EB51-42B6-B412-5D8C58707E98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-150" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4272" yWindow="2568" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BattleLevelConfig" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -142,10 +141,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>1002,1002,1002</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>战斗胜利获取的经验值</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -163,6 +158,10 @@
   </si>
   <si>
     <t>c</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>1002,1003,1004</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -256,7 +255,7 @@
     <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -566,25 +565,25 @@
   <dimension ref="C2:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.2" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="12.75" style="2" customWidth="1"/>
-    <col min="3" max="4" width="12.625" style="2" customWidth="1"/>
-    <col min="5" max="6" width="13.375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="18.5" style="2" customWidth="1"/>
+    <col min="1" max="1" width="21.109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="12.77734375" style="2" customWidth="1"/>
+    <col min="3" max="4" width="12.6640625" style="2" customWidth="1"/>
+    <col min="5" max="6" width="13.33203125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="18.44140625" style="2" customWidth="1"/>
     <col min="8" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="3:7" ht="14.25" x14ac:dyDescent="0.3">
       <c r="E2" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="3:7" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="3:7" ht="14.25" x14ac:dyDescent="0.3">
       <c r="C3" s="3" t="s">
         <v>0</v>
       </c>
@@ -592,16 +591,16 @@
         <v>14</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>20</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="3:7" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="3:7" ht="14.25" x14ac:dyDescent="0.3">
       <c r="C4" s="3" t="s">
         <v>0</v>
       </c>
@@ -615,10 +614,10 @@
         <v>16</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="3:7" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="3:7" ht="14.25" x14ac:dyDescent="0.3">
       <c r="C5" s="3" t="s">
         <v>2</v>
       </c>
@@ -632,15 +631,15 @@
         <v>15</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.15">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C6" s="1">
         <v>1</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>4</v>
@@ -652,7 +651,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:7" ht="14.25" x14ac:dyDescent="0.3">
       <c r="C7" s="1">
         <v>2</v>
       </c>
@@ -669,7 +668,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:7" ht="14.25" x14ac:dyDescent="0.3">
       <c r="C8" s="1">
         <v>3</v>
       </c>
@@ -686,7 +685,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:7" ht="14.25" x14ac:dyDescent="0.3">
       <c r="C9" s="1">
         <v>4</v>
       </c>
@@ -703,7 +702,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="3:7" ht="14.25" x14ac:dyDescent="0.3">
       <c r="C10" s="1">
         <v>5</v>
       </c>
@@ -720,7 +719,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="3:7" ht="14.25" x14ac:dyDescent="0.3">
       <c r="C11" s="1">
         <v>6</v>
       </c>
@@ -737,7 +736,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="3:7" ht="14.25" x14ac:dyDescent="0.3">
       <c r="C12" s="1">
         <v>7</v>
       </c>
@@ -754,7 +753,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:7" ht="14.25" x14ac:dyDescent="0.3">
       <c r="C13" s="1">
         <v>8</v>
       </c>
@@ -771,7 +770,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:7" ht="14.25" x14ac:dyDescent="0.3">
       <c r="C14" s="1">
         <v>9</v>
       </c>
@@ -788,7 +787,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="3:7" ht="14.25" x14ac:dyDescent="0.3">
       <c r="C15" s="1">
         <v>10</v>
       </c>
@@ -805,7 +804,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="3:7" ht="14.25" x14ac:dyDescent="0.3">
       <c r="C16" s="1">
         <v>11</v>
       </c>
@@ -822,7 +821,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:7" ht="14.25" x14ac:dyDescent="0.3">
       <c r="C17" s="1">
         <v>12</v>
       </c>
@@ -842,6 +841,6 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>